<commit_message>
Aoache POI Cucumber kardeşliği
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber_Kursu5\src\test\java\ApachePOI\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber6\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -63,52 +63,52 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulis111</t>
-  </si>
-  <si>
-    <t>ulis112</t>
-  </si>
-  <si>
-    <t>ulis113</t>
-  </si>
-  <si>
-    <t>ulis114</t>
-  </si>
-  <si>
-    <t>ulis115</t>
-  </si>
-  <si>
-    <t>ulis116</t>
-  </si>
-  <si>
-    <t>ulis117</t>
-  </si>
-  <si>
-    <t>ulis118</t>
-  </si>
-  <si>
-    <t>ubs111</t>
-  </si>
-  <si>
-    <t>ubs112</t>
-  </si>
-  <si>
-    <t>ubs113</t>
-  </si>
-  <si>
-    <t>ubs114</t>
-  </si>
-  <si>
-    <t>ubs115</t>
-  </si>
-  <si>
-    <t>ubs116</t>
-  </si>
-  <si>
-    <t>ubs117</t>
-  </si>
-  <si>
-    <t>ubs118</t>
+    <t>ulis1111</t>
+  </si>
+  <si>
+    <t>ulis1122</t>
+  </si>
+  <si>
+    <t>ulis1133</t>
+  </si>
+  <si>
+    <t>ulis1144</t>
+  </si>
+  <si>
+    <t>ulis1154</t>
+  </si>
+  <si>
+    <t>ulis1164</t>
+  </si>
+  <si>
+    <t>ulis1174</t>
+  </si>
+  <si>
+    <t>ulis1184</t>
+  </si>
+  <si>
+    <t>ubs13</t>
+  </si>
+  <si>
+    <t>ubs141</t>
+  </si>
+  <si>
+    <t>ubs152</t>
+  </si>
+  <si>
+    <t>ubs162</t>
+  </si>
+  <si>
+    <t>ubs172</t>
+  </si>
+  <si>
+    <t>ubs182</t>
+  </si>
+  <si>
+    <t>ubs192</t>
+  </si>
+  <si>
+    <t>ubs202</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>